<commit_message>
PDF für Blatt 3
</commit_message>
<xml_diff>
--- a/RA/blatt03/Messungen_Blatt_3.xlsx
+++ b/RA/blatt03/Messungen_Blatt_3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Dhrystones/Sec</t>
   </si>
@@ -45,10 +45,13 @@
     <t>20302507.4</t>
   </si>
   <si>
-    <t xml:space="preserve">60000 - 800000 </t>
-  </si>
-  <si>
-    <t>ist normaler Wert für heutige Desktop-PCs</t>
+    <t xml:space="preserve">60000 - 80000 </t>
+  </si>
+  <si>
+    <t>heutige Desktop-PCs</t>
+  </si>
+  <si>
+    <t>ist normaler Wert für</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -415,6 +418,7 @@
         <v>1</v>
       </c>
       <c r="D3">
+        <f>AVERAGE(A2:A6)</f>
         <v>76923</v>
       </c>
       <c r="F3" t="s">
@@ -429,6 +433,7 @@
         <v>2</v>
       </c>
       <c r="D4">
+        <f>VAR(A2:A6)</f>
         <v>0</v>
       </c>
     </row>
@@ -460,7 +465,8 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>138.504155</v>
+        <f>AVERAGE(A9:A13)</f>
+        <v>138.5233518</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -471,7 +477,8 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <f>VAR(A9:A13)</f>
+        <v>1.8425856512005992E-3</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -497,31 +504,46 @@
         <v>106.95187199999999</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>106.89470900000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <f>AVERAGE(A16:A20)</f>
+        <v>106.9290068</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>106.89470900000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="D18">
+        <f>VAR(A16:A20)</f>
+        <v>9.8028257069960657E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>106.95187199999999</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>106.95187199999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>